<commit_message>
With large book list, still before dictionary dates
</commit_message>
<xml_diff>
--- a/Data/data.xlsx
+++ b/Data/data.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="4020" yWindow="1540" windowWidth="25600" windowHeight="14180" tabRatio="500"/>
+    <workbookView xWindow="1020" yWindow="460" windowWidth="25600" windowHeight="14180" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="21">
   <si>
     <t>adambede</t>
   </si>
@@ -53,9 +53,6 @@
     <t>Roughing It</t>
   </si>
   <si>
-    <t>The Gilded Age</t>
-  </si>
-  <si>
     <t>The Adventures of Tom Sawyer</t>
   </si>
   <si>
@@ -72,6 +69,27 @@
   </si>
   <si>
     <t>http://mark-twain.classic-literature.co.uk/</t>
+  </si>
+  <si>
+    <t>https://en.wikipedia.org/wiki/Henry_James_bibliography#Novels</t>
+  </si>
+  <si>
+    <t>theamericans</t>
+  </si>
+  <si>
+    <t>theeuropeans</t>
+  </si>
+  <si>
+    <t>confidence</t>
+  </si>
+  <si>
+    <t>portraitofaladyvol1</t>
+  </si>
+  <si>
+    <t>portraitofaladyvol2</t>
+  </si>
+  <si>
+    <t>thegoldenbowl</t>
   </si>
 </sst>
 </file>
@@ -386,10 +404,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D14"/>
+  <dimension ref="A1:D18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8:A14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -413,13 +431,36 @@
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4">
+        <v>1871</v>
+      </c>
       <c r="C4" t="s">
         <v>2</v>
       </c>
     </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5">
+        <v>1877</v>
+      </c>
+      <c r="C5" t="s">
+        <v>15</v>
+      </c>
+    </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6">
+        <v>1878</v>
+      </c>
       <c r="C6" t="s">
-        <v>3</v>
+        <v>16</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
@@ -427,10 +468,10 @@
         <v>14</v>
       </c>
       <c r="B7">
-        <v>1869</v>
+        <v>1879</v>
       </c>
       <c r="C7" t="s">
-        <v>4</v>
+        <v>17</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
@@ -438,10 +479,10 @@
         <v>14</v>
       </c>
       <c r="B8">
-        <v>1872</v>
+        <v>1881</v>
       </c>
       <c r="C8" t="s">
-        <v>7</v>
+        <v>18</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
@@ -449,65 +490,103 @@
         <v>14</v>
       </c>
       <c r="B9">
-        <v>1873</v>
+        <v>1881</v>
       </c>
       <c r="C9" t="s">
-        <v>8</v>
+        <v>19</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>14</v>
       </c>
-      <c r="B10">
-        <v>1876</v>
-      </c>
       <c r="C10" t="s">
-        <v>9</v>
+        <v>20</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>14</v>
       </c>
-      <c r="B11">
-        <v>1883</v>
-      </c>
       <c r="C11" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B12">
-        <v>1889</v>
+        <v>1869</v>
       </c>
       <c r="C12" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B13">
-        <v>1894</v>
+        <v>1872</v>
       </c>
       <c r="C13" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B14">
+        <v>1876</v>
+      </c>
+      <c r="C14" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>13</v>
+      </c>
+      <c r="B15">
+        <v>1883</v>
+      </c>
+      <c r="C15" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>13</v>
+      </c>
+      <c r="B16">
+        <v>1889</v>
+      </c>
+      <c r="C16" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>13</v>
+      </c>
+      <c r="B17">
+        <v>1894</v>
+      </c>
+      <c r="C17" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>13</v>
+      </c>
+      <c r="B18">
         <v>1896</v>
       </c>
-      <c r="C14" t="s">
-        <v>13</v>
+      <c r="C18" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>